<commit_message>
Versão 20250613 - Revisão 00 para entrega.
</commit_message>
<xml_diff>
--- a/dataset_pv_nafta.xlsx
+++ b/dataset_pv_nafta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petrobrasbr-my.sharepoint.com/personal/fdamata_petrobras_com_br/Documents/Documents/Pessoal/Projetos IA/pucrj/cda_fma/mvp-analise-de-dados-e-boas-praticas/mvp_sprint_01_FMA_2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{16C9A5C1-A3A7-4EFC-BC36-C693C97414CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9F6ECDC-1F1C-4CBC-8BAD-1D0731CA682E}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{16C9A5C1-A3A7-4EFC-BC36-C693C97414CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{134231A0-D8C6-408A-8ABC-2D99D2953F27}"/>
   <bookViews>
-    <workbookView xWindow="20280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8C706EEA-6AFF-40CF-98B4-7F12082183C5}"/>
+    <workbookView xWindow="28680" yWindow="-30" windowWidth="24240" windowHeight="13020" xr2:uid="{8C706EEA-6AFF-40CF-98B4-7F12082183C5}"/>
   </bookViews>
   <sheets>
     <sheet name="pv_nafta" sheetId="1" r:id="rId1"/>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86164CC1-C2F7-4587-8400-9C103BB4EE5C}">
   <dimension ref="A1:S1817"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R114" sqref="R114"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>